<commit_message>
Added payload generation logic for the AR parsed data
</commit_message>
<xml_diff>
--- a/data/input/AR_input.xlsx
+++ b/data/input/AR_input.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="13">
   <si>
     <t>Table 1</t>
   </si>
@@ -25,10 +25,16 @@
     <t>address</t>
   </si>
   <si>
+    <t>notes</t>
+  </si>
+  <si>
     <t>shashwat</t>
   </si>
   <si>
     <t>Kalkaji</t>
+  </si>
+  <si>
+    <t>First note</t>
   </si>
   <si>
     <t>rohit</t>
@@ -41,6 +47,9 @@
   </si>
   <si>
     <t>Mumbai</t>
+  </si>
+  <si>
+    <t>Second note</t>
   </si>
 </sst>
 </file>
@@ -1335,61 +1344,77 @@
       <c r="C2" t="s" s="3">
         <v>3</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" t="s" s="3">
+        <v>4</v>
+      </c>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
       <c r="A3" t="s" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="6">
         <v>123</v>
       </c>
       <c r="C3" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="D3" s="8"/>
+        <v>6</v>
+      </c>
+      <c r="D3" t="s" s="7">
+        <v>7</v>
+      </c>
       <c r="E3" s="8"/>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
       <c r="A4" t="s" s="9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" s="10">
         <v>234</v>
       </c>
       <c r="C4" t="s" s="11">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s" s="11">
         <v>7</v>
       </c>
-      <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
       <c r="A5" t="s" s="9">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="10">
         <v>345</v>
       </c>
       <c r="C5" t="s" s="11">
-        <v>9</v>
-      </c>
-      <c r="D5" s="12"/>
+        <v>11</v>
+      </c>
+      <c r="D5" t="s" s="11">
+        <v>7</v>
+      </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="13"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
+      <c r="A6" t="s" s="9">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10">
+        <v>123</v>
+      </c>
+      <c r="C6" t="s" s="11">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s" s="11">
+        <v>12</v>
+      </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>

</xml_diff>